<commit_message>
Add GHG files to github
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Raw_GHG/data/GC 20240326.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Raw_GHG/data/GC 20240326.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\StreamTeam Analytical Lab\Projects\Carey Misc\2024 season misc analyses\GC 2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abreefpilz\Documents\GitHub\Reservoirs2\Data\DataNotYetUploadedToEDI\Raw_GHG\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C4A67E3-A103-4C3F-AC21-8FC79B9A6CA3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2573957C-322C-4110-815F-091A2878EE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11310" windowHeight="11450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serum CH4 CO2" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="58">
   <si>
     <t>Data#</t>
   </si>
@@ -193,7 +204,7 @@
     <t>actually spiked?</t>
   </si>
   <si>
-    <t>leaky</t>
+    <t>leaked during HS creation</t>
   </si>
 </sst>
 </file>
@@ -1062,19 +1073,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A7:BU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AP46" sqref="AP46"/>
+    <sheetView tabSelected="1" topLeftCell="AC18" workbookViewId="0">
+      <selection activeCell="AV29" sqref="AV29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="23.54296875" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="31" max="31" width="21.453125" customWidth="1"/>
-    <col min="60" max="60" width="8.7265625" style="9"/>
+    <col min="2" max="2" width="23.5234375" customWidth="1"/>
+    <col min="3" max="3" width="17.7890625" customWidth="1"/>
+    <col min="31" max="31" width="21.47265625" customWidth="1"/>
+    <col min="60" max="60" width="8.734375" style="9"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1088,7 +1099,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:73" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:73" ht="129.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1287,7 +1298,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>48</v>
       </c>
@@ -1494,7 +1505,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>49</v>
       </c>
@@ -1698,7 +1709,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>50</v>
       </c>
@@ -1902,7 +1913,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>51</v>
       </c>
@@ -2106,7 +2117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <v>52</v>
       </c>
@@ -2310,7 +2321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <v>53</v>
       </c>
@@ -2514,7 +2525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <v>54</v>
       </c>
@@ -2718,7 +2729,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <v>55</v>
       </c>
@@ -2922,7 +2933,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <v>56</v>
       </c>
@@ -3126,7 +3137,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <v>57</v>
       </c>
@@ -3330,7 +3341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <v>58</v>
       </c>
@@ -3534,7 +3545,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <v>59</v>
       </c>
@@ -3738,7 +3749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <v>60</v>
       </c>
@@ -3942,7 +3953,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <v>61</v>
       </c>
@@ -4146,7 +4157,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <v>62</v>
       </c>
@@ -4350,7 +4361,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <v>63</v>
       </c>
@@ -4554,7 +4565,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <v>64</v>
       </c>
@@ -4758,7 +4769,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <v>65</v>
       </c>
@@ -4962,7 +4973,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <v>66</v>
       </c>
@@ -5166,7 +5177,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <v>67</v>
       </c>
@@ -5370,7 +5381,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:73" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:73" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <v>68</v>
       </c>
@@ -5380,8 +5391,8 @@
       <c r="C29" s="2">
         <v>45377.893310185187</v>
       </c>
-      <c r="D29" t="s">
-        <v>55</v>
+      <c r="D29">
+        <v>172</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
@@ -5419,8 +5430,8 @@
       <c r="Q29" s="2">
         <v>45377.893310185187</v>
       </c>
-      <c r="R29" t="s">
-        <v>55</v>
+      <c r="R29">
+        <v>172</v>
       </c>
       <c r="S29" t="s">
         <v>13</v>
@@ -5458,8 +5469,8 @@
       <c r="AE29" s="2">
         <v>45377.893310185187</v>
       </c>
-      <c r="AF29" t="s">
-        <v>55</v>
+      <c r="AF29">
+        <v>172</v>
       </c>
       <c r="AG29" t="s">
         <v>13</v>

</xml_diff>